<commit_message>
PROS-13075 - CCRU - POS 2020 KPIs - correction
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2020/POS_VALIDATION/PoS 2020 List.xlsx
+++ b/Projects/CCRU/Data/KPIs_2020/POS_VALIDATION/PoS 2020 List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PoS List" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,37 +31,37 @@
     <t xml:space="preserve">Sheet_in</t>
   </si>
   <si>
+    <t xml:space="preserve">File_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet_out SPLIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File_in SPLIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet_in SPLIT</t>
+  </si>
+  <si>
     <t xml:space="preserve">File_out MERGED</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheet_out SPLIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File_in SPLIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheet_in SPLIT</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoS 2020 - FT - CITIES PG</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2020 - FT.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FT - CITIES PG</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2020 - ALL.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2020 - FT.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FT - CITIES PG</t>
   </si>
   <si>
     <t xml:space="preserve">PoS 2020 - FT - CITIES SBI</t>
@@ -575,20 +575,20 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.7908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.18877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3724489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.8367346938775"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,14 +639,14 @@
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f aca="false">CONCATENATE(G2,".xlsx")</f>
+      <c r="G2" s="2" t="str">
+        <f aca="false">CONCATENATE(F2,".xlsx")</f>
         <v>FT - CITIES PG.xlsx</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -665,16 +665,16 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="str">
-        <f aca="false">CONCATENATE(G3,".xlsx")</f>
+      <c r="G3" s="2" t="str">
+        <f aca="false">CONCATENATE(F3,".xlsx")</f>
         <v>FT - CITIES SBI.xlsx</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -693,16 +693,16 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="str">
-        <f aca="false">CONCATENATE(G4,".xlsx")</f>
+      <c r="G4" s="2" t="str">
+        <f aca="false">CONCATENATE(F4,".xlsx")</f>
         <v>FT - REG PG.xlsx</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -721,16 +721,16 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="str">
-        <f aca="false">CONCATENATE(G5,".xlsx")</f>
+      <c r="G5" s="2" t="str">
+        <f aca="false">CONCATENATE(F5,".xlsx")</f>
         <v>FT - REG SBI.xlsx</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -749,16 +749,16 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="2" t="str">
-        <f aca="false">CONCATENATE(G6,".xlsx")</f>
+      <c r="G6" s="2" t="str">
+        <f aca="false">CONCATENATE(F6,".xlsx")</f>
         <v>FT - SOUTH PG.xlsx</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -777,16 +777,16 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="2" t="str">
-        <f aca="false">CONCATENATE(G7,".xlsx")</f>
+      <c r="G7" s="2" t="str">
+        <f aca="false">CONCATENATE(F7,".xlsx")</f>
         <v>FT - SOUTH SBI.xlsx</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -805,16 +805,16 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2" t="str">
-        <f aca="false">CONCATENATE(G8,".xlsx")</f>
+      <c r="G8" s="2" t="str">
+        <f aca="false">CONCATENATE(F8,".xlsx")</f>
         <v>FT - USFE PG.xlsx</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -833,16 +833,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="2" t="str">
-        <f aca="false">CONCATENATE(G9,".xlsx")</f>
+      <c r="G9" s="2" t="str">
+        <f aca="false">CONCATENATE(F9,".xlsx")</f>
         <v>FT - USFE SBI.xlsx</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -861,16 +861,16 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2" t="str">
-        <f aca="false">CONCATENATE(G10,".xlsx")</f>
+      <c r="G10" s="2" t="str">
+        <f aca="false">CONCATENATE(F10,".xlsx")</f>
         <v>FT S - Beer.xlsx</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -889,16 +889,16 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="2" t="str">
-        <f aca="false">CONCATENATE(G11,".xlsx")</f>
+      <c r="G11" s="2" t="str">
+        <f aca="false">CONCATENATE(F11,".xlsx")</f>
         <v>FT S - Bread.xlsx</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -917,16 +917,16 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="2" t="str">
-        <f aca="false">CONCATENATE(G12,".xlsx")</f>
+      <c r="G12" s="2" t="str">
+        <f aca="false">CONCATENATE(F12,".xlsx")</f>
         <v>FT S - Dairy.xlsx</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -945,16 +945,16 @@
         <v>11</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="2" t="str">
-        <f aca="false">CONCATENATE(G13,".xlsx")</f>
+      <c r="G13" s="2" t="str">
+        <f aca="false">CONCATENATE(F13,".xlsx")</f>
         <v>FT S - Meat.xlsx</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -973,16 +973,16 @@
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="2" t="str">
-        <f aca="false">CONCATENATE(G14,".xlsx")</f>
+      <c r="G14" s="2" t="str">
+        <f aca="false">CONCATENATE(F14,".xlsx")</f>
         <v>FT S - Sweets.xlsx</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
@@ -1001,16 +1001,16 @@
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="2" t="str">
-        <f aca="false">CONCATENATE(G15,".xlsx")</f>
+      <c r="G15" s="2" t="str">
+        <f aca="false">CONCATENATE(F15,".xlsx")</f>
         <v>FT S - Tobacco.xlsx</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -1029,1024 +1029,1024 @@
         <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="2" t="str">
-        <f aca="false">CONCATENATE(G16,".xlsx")</f>
+      <c r="G16" s="2" t="str">
+        <f aca="false">CONCATENATE(F16,".xlsx")</f>
         <v>FT S - Veggies.xlsx</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="3" t="str">
-        <f aca="false">CONCATENATE(G17,".xlsx")</f>
+      <c r="G17" s="3" t="str">
+        <f aca="false">CONCATENATE(F17,".xlsx")</f>
         <v>MT ConvBig - CAP.xlsx</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="3" t="str">
-        <f aca="false">CONCATENATE(G18,".xlsx")</f>
+      <c r="G18" s="3" t="str">
+        <f aca="false">CONCATENATE(F18,".xlsx")</f>
         <v>MT ConvSmall - CAP.xlsx</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="3" t="str">
-        <f aca="false">CONCATENATE(G19,".xlsx")</f>
+      <c r="G19" s="3" t="str">
+        <f aca="false">CONCATENATE(F19,".xlsx")</f>
         <v>MT Hypermarket - CAP.xlsx</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="3" t="str">
-        <f aca="false">CONCATENATE(G20,".xlsx")</f>
+      <c r="G20" s="3" t="str">
+        <f aca="false">CONCATENATE(F20,".xlsx")</f>
         <v>MT Supermarket - CAP.xlsx</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="3" t="str">
-        <f aca="false">CONCATENATE(G21,".xlsx")</f>
+      <c r="G21" s="3" t="str">
+        <f aca="false">CONCATENATE(F21,".xlsx")</f>
         <v>MT ConvBig - REG.xlsx</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="3" t="str">
-        <f aca="false">CONCATENATE(G22,".xlsx")</f>
+      <c r="G22" s="3" t="str">
+        <f aca="false">CONCATENATE(F22,".xlsx")</f>
         <v>MT ConvSmall - REG.xlsx</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="3" t="str">
-        <f aca="false">CONCATENATE(G23,".xlsx")</f>
+      <c r="G23" s="3" t="str">
+        <f aca="false">CONCATENATE(F23,".xlsx")</f>
         <v>MT Hypermarket - REG.xlsx</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="3" t="str">
-        <f aca="false">CONCATENATE(G24,".xlsx")</f>
+      <c r="G24" s="3" t="str">
+        <f aca="false">CONCATENATE(F24,".xlsx")</f>
         <v>MT Supermarket - REG.xlsx</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="3" t="str">
-        <f aca="false">CONCATENATE(G25,".xlsx")</f>
+      <c r="G25" s="3" t="str">
+        <f aca="false">CONCATENATE(F25,".xlsx")</f>
         <v>MT ConvBig - NKA.xlsx</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="3" t="str">
-        <f aca="false">CONCATENATE(G26,".xlsx")</f>
+      <c r="G26" s="3" t="str">
+        <f aca="false">CONCATENATE(F26,".xlsx")</f>
         <v>MT ConvSmall - NKA.xlsx</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="3" t="str">
-        <f aca="false">CONCATENATE(G27,".xlsx")</f>
+      <c r="G27" s="3" t="str">
+        <f aca="false">CONCATENATE(F27,".xlsx")</f>
         <v>MT Hypermarket - NKA.xlsx</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H28" s="3" t="str">
-        <f aca="false">CONCATENATE(G28,".xlsx")</f>
+      <c r="G28" s="3" t="str">
+        <f aca="false">CONCATENATE(F28,".xlsx")</f>
         <v>MT Supermarket - NKA.xlsx</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H29" s="4" t="str">
-        <f aca="false">CONCATENATE(G29,".xlsx")</f>
+      <c r="G29" s="4" t="str">
+        <f aca="false">CONCATENATE(F29,".xlsx")</f>
         <v>IC BarNightClub.xlsx</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="4" t="str">
-        <f aca="false">CONCATENATE(G30,".xlsx")</f>
+      <c r="G30" s="4" t="str">
+        <f aca="false">CONCATENATE(F30,".xlsx")</f>
         <v>IC Canteen - ATW.xlsx</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="4" t="str">
-        <f aca="false">CONCATENATE(G31,".xlsx")</f>
+      <c r="G31" s="4" t="str">
+        <f aca="false">CONCATENATE(F31,".xlsx")</f>
         <v>IC Canteen - EDU.xlsx</v>
       </c>
-      <c r="I31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H32" s="4" t="str">
-        <f aca="false">CONCATENATE(G32,".xlsx")</f>
+      <c r="G32" s="4" t="str">
+        <f aca="false">CONCATENATE(F32,".xlsx")</f>
         <v>IC Cinema.xlsx</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H33" s="4" t="str">
-        <f aca="false">CONCATENATE(G33,".xlsx")</f>
+      <c r="G33" s="4" t="str">
+        <f aca="false">CONCATENATE(F33,".xlsx")</f>
         <v>IC CoffeeShop.xlsx</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H34" s="4" t="str">
-        <f aca="false">CONCATENATE(G34,".xlsx")</f>
+      <c r="G34" s="4" t="str">
+        <f aca="false">CONCATENATE(F34,".xlsx")</f>
         <v>IC RestCafe.xlsx</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H35" s="4" t="str">
-        <f aca="false">CONCATENATE(G35,".xlsx")</f>
+      <c r="G35" s="4" t="str">
+        <f aca="false">CONCATENATE(F35,".xlsx")</f>
         <v>IC FastFood.xlsx</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="4" t="str">
-        <f aca="false">CONCATENATE(G36,".xlsx")</f>
+      <c r="G36" s="4" t="str">
+        <f aca="false">CONCATENATE(F36,".xlsx")</f>
         <v>IC Petrol - Kiosk.xlsx</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H37" s="4" t="str">
-        <f aca="false">CONCATENATE(G37,".xlsx")</f>
+      <c r="G37" s="4" t="str">
+        <f aca="false">CONCATENATE(F37,".xlsx")</f>
         <v>IC Petrol - Medium.xlsx</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H38" s="4" t="str">
-        <f aca="false">CONCATENATE(G38,".xlsx")</f>
+      <c r="G38" s="4" t="str">
+        <f aca="false">CONCATENATE(F38,".xlsx")</f>
         <v>IC Petrol - Large.xlsx</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H39" s="4" t="str">
-        <f aca="false">CONCATENATE(G39,".xlsx")</f>
+      <c r="G39" s="4" t="str">
+        <f aca="false">CONCATENATE(F39,".xlsx")</f>
         <v>IC QSR - FoodCourt.xlsx</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H40" s="4" t="str">
-        <f aca="false">CONCATENATE(G40,".xlsx")</f>
+      <c r="G40" s="4" t="str">
+        <f aca="false">CONCATENATE(F40,".xlsx")</f>
         <v>IC QSR - Classic.xlsx</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="4" t="str">
-        <f aca="false">CONCATENATE(G41,".xlsx")</f>
+      <c r="G41" s="4" t="str">
+        <f aca="false">CONCATENATE(F41,".xlsx")</f>
         <v>IC QSR - GastroMarket.xlsx</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="4" t="str">
-        <f aca="false">CONCATENATE(G42,".xlsx")</f>
+      <c r="G42" s="4" t="str">
+        <f aca="false">CONCATENATE(F42,".xlsx")</f>
         <v>IC Vending - Airport.xlsx</v>
       </c>
-      <c r="I42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H43" s="4" t="str">
-        <f aca="false">CONCATENATE(G43,".xlsx")</f>
+      <c r="G43" s="4" t="str">
+        <f aca="false">CONCATENATE(F43,".xlsx")</f>
         <v>IC Vending - Transportation.xlsx</v>
       </c>
-      <c r="I43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H44" s="4" t="str">
-        <f aca="false">CONCATENATE(G44,".xlsx")</f>
+      <c r="G44" s="4" t="str">
+        <f aca="false">CONCATENATE(F44,".xlsx")</f>
         <v>IC Vending - AtWork.xlsx</v>
       </c>
-      <c r="I44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H45" s="4" t="str">
-        <f aca="false">CONCATENATE(G45,".xlsx")</f>
+      <c r="G45" s="4" t="str">
+        <f aca="false">CONCATENATE(F45,".xlsx")</f>
         <v>IC Vending - University.xlsx</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H46" s="4" t="str">
-        <f aca="false">CONCATENATE(G46,".xlsx")</f>
+      <c r="G46" s="4" t="str">
+        <f aca="false">CONCATENATE(F46,".xlsx")</f>
         <v>IC NonGroceryShop.xlsx</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H47" s="4" t="str">
-        <f aca="false">CONCATENATE(G47,".xlsx")</f>
+      <c r="G47" s="4" t="str">
+        <f aca="false">CONCATENATE(F47,".xlsx")</f>
         <v>IC Fitness.xlsx</v>
       </c>
-      <c r="I47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H48" s="4" t="str">
-        <f aca="false">CONCATENATE(G48,".xlsx")</f>
+      <c r="G48" s="4" t="str">
+        <f aca="false">CONCATENATE(F48,".xlsx")</f>
         <v>IC Beauty.xlsx</v>
       </c>
-      <c r="I48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H49" s="4" t="str">
-        <f aca="false">CONCATENATE(G49,".xlsx")</f>
+      <c r="G49" s="4" t="str">
+        <f aca="false">CONCATENATE(F49,".xlsx")</f>
         <v>IC DrugStore.xlsx</v>
       </c>
-      <c r="I49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H50" s="4" t="str">
-        <f aca="false">CONCATENATE(G50,".xlsx")</f>
+      <c r="G50" s="4" t="str">
+        <f aca="false">CONCATENATE(F50,".xlsx")</f>
         <v>IC KioskOTG.xlsx</v>
       </c>
-      <c r="I50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H51" s="4" t="str">
-        <f aca="false">CONCATENATE(G51,".xlsx")</f>
+      <c r="G51" s="4" t="str">
+        <f aca="false">CONCATENATE(F51,".xlsx")</f>
         <v>IC CartMobile.xlsx</v>
       </c>
-      <c r="I51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H52" s="4" t="str">
-        <f aca="false">CONCATENATE(G52,".xlsx")</f>
+      <c r="G52" s="4" t="str">
+        <f aca="false">CONCATENATE(F52,".xlsx")</f>
         <v>IC CoffeePoint.xlsx</v>
       </c>
-      <c r="I52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>